<commit_message>
docs: terminate third sprint
</commit_message>
<xml_diff>
--- a/docs/process/third-sprint-backlog.xlsx
+++ b/docs/process/third-sprint-backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t xml:space="preserve">Remaining effort at the end of the day ... </t>
   </si>
@@ -34,16 +34,16 @@
     <t>Configurazione di SCoverage</t>
   </si>
   <si>
-    <t>?</t>
+    <t>Felice</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
   <si>
     <t>L'utente deve poter avviare una partita impostando una configurazione iniziale</t>
   </si>
   <si>
     <t>Sviluppo del modello della configurazione</t>
-  </si>
-  <si>
-    <t>Felice</t>
   </si>
   <si>
     <t>Modifica della pagina di configurazione della partita in base al modello</t>
@@ -638,8 +638,12 @@
       <c r="E4" s="12">
         <v>2.0</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13"/>
+      <c r="F4" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
@@ -656,20 +660,26 @@
     <row r="5">
       <c r="A5" s="9"/>
       <c r="B5" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5" s="12">
         <v>3.0</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="F5" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G5" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
@@ -689,15 +699,23 @@
         <v>11</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6" s="12">
         <v>4.0</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
+      <c r="F6" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="G6" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="H6" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
@@ -723,13 +741,27 @@
       <c r="E7" s="12">
         <v>6.0</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
+      <c r="F7" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="G7" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="H7" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="I7" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="J7" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="K7" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
@@ -750,13 +782,23 @@
       <c r="E8" s="12">
         <v>2.0</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
+      <c r="F8" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="H8" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
+      <c r="L8" s="12"/>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
@@ -777,13 +819,27 @@
       <c r="E9" s="12">
         <v>6.0</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="F9" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="G9" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="H9" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="I9" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="J9" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="K9" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
       <c r="O9" s="14"/>
@@ -804,13 +860,27 @@
       <c r="E10" s="12">
         <v>1.0</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="F10" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="G10" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="H10" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I10" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="J10" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="K10" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
       <c r="O10" s="14"/>
@@ -833,7 +903,9 @@
       <c r="E11" s="12">
         <v>2.0</v>
       </c>
-      <c r="F11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -860,8 +932,12 @@
       <c r="E12" s="12">
         <v>3.0</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="F12" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="13"/>
@@ -887,10 +963,18 @@
       <c r="E13" s="12">
         <v>3.0</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="F13" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H13" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="13"/>
@@ -916,11 +1000,21 @@
       <c r="E14" s="12">
         <v>4.0</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="F14" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="H14" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="I14" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="K14" s="12"/>
       <c r="L14" s="13"/>
       <c r="M14" s="14"/>
@@ -943,11 +1037,21 @@
       <c r="E15" s="12">
         <v>1.0</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
+      <c r="F15" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="G15" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="H15" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I15" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="K15" s="12"/>
       <c r="L15" s="13"/>
       <c r="M15" s="14"/>
@@ -965,17 +1069,29 @@
         <v>26</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E16" s="12">
         <v>1.0</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="F16" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="G16" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="H16" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I16" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="L16" s="12"/>
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
@@ -992,17 +1108,29 @@
         <v>27</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E17" s="12">
         <v>3.0</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
+      <c r="F17" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G17" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H17" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I17" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J17" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="L17" s="12"/>
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>

</xml_diff>